<commit_message>
Predicting PM10 hourly levels / Organizing Data Gathering and Exploration code
</commit_message>
<xml_diff>
--- a/arima_prediction_graph.xlsx
+++ b/arima_prediction_graph.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/507d04ca7be29483/00_master_data_science/TFM_KSchool_Gijon_Air_Pollution/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SErgio\OneDrive\00_master_data_science\TFM_KSchool_Gijon_Air_Pollution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F038860C-ADCD-483E-99F6-B8624C407276}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="8_{F038860C-ADCD-483E-99F6-B8624C407276}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{B75EF87B-DF3F-4B5A-953E-D63ED53A25C8}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="1910" windowHeight="0" xr2:uid="{25F250B0-3884-4528-9D34-9580BA324527}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="1910" windowHeight="0" activeTab="1" xr2:uid="{25F250B0-3884-4528-9D34-9580BA324527}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="arima_graph" sheetId="1" r:id="rId1"/>
+    <sheet name="pm10_limits" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>year_month</t>
   </si>
@@ -40,6 +41,30 @@
   </si>
   <si>
     <t>real 2017</t>
+  </si>
+  <si>
+    <t>ue</t>
+  </si>
+  <si>
+    <t>oms</t>
+  </si>
+  <si>
+    <t>Promedio 24 horas</t>
+  </si>
+  <si>
+    <t>&lt;= 50 ug/m3; &lt;= 35 días</t>
+  </si>
+  <si>
+    <t>&lt;= 50 ug/m3; &lt;= 3 días</t>
+  </si>
+  <si>
+    <t>Promedio anual</t>
+  </si>
+  <si>
+    <t>&lt;= 40 ug/m3</t>
+  </si>
+  <si>
+    <t>&lt;= 20 ug/m3</t>
   </si>
 </sst>
 </file>
@@ -88,7 +113,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -98,6 +123,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -171,7 +199,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
+              <c:f>arima_graph!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -194,7 +222,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$13</c:f>
+              <c:f>arima_graph!$B$2:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -249,7 +277,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>arima_graph!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -272,7 +300,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$13</c:f>
+              <c:f>arima_graph!$C$2:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -1414,7 +1442,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F50DCA78-E89A-4BA6-97A1-F445FBB88E11}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
@@ -1569,4 +1597,54 @@
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8264788F-3ED7-499F-95A3-F67646295472}">
+  <dimension ref="E4:G6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="5" max="5" width="19.1796875" customWidth="1"/>
+    <col min="6" max="6" width="20.86328125" customWidth="1"/>
+    <col min="7" max="7" width="22.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="5:7" x14ac:dyDescent="0.75">
+      <c r="F4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="5:7" x14ac:dyDescent="0.75">
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="5:7" x14ac:dyDescent="0.75">
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "Predicting PM10 hourly levels / Organizing Data Gathering and Exploration code"
This reverts commit be50319e493d65c465c7444cce88315e3c50b432.
</commit_message>
<xml_diff>
--- a/arima_prediction_graph.xlsx
+++ b/arima_prediction_graph.xlsx
@@ -5,16 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SErgio\OneDrive\00_master_data_science\TFM_KSchool_Gijon_Air_Pollution\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/507d04ca7be29483/00_master_data_science/TFM_KSchool_Gijon_Air_Pollution/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="8_{F038860C-ADCD-483E-99F6-B8624C407276}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{B75EF87B-DF3F-4B5A-953E-D63ED53A25C8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F038860C-ADCD-483E-99F6-B8624C407276}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="1910" windowHeight="0" activeTab="1" xr2:uid="{25F250B0-3884-4528-9D34-9580BA324527}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="1910" windowHeight="0" xr2:uid="{25F250B0-3884-4528-9D34-9580BA324527}"/>
   </bookViews>
   <sheets>
-    <sheet name="arima_graph" sheetId="1" r:id="rId1"/>
-    <sheet name="pm10_limits" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>year_month</t>
   </si>
@@ -41,30 +40,6 @@
   </si>
   <si>
     <t>real 2017</t>
-  </si>
-  <si>
-    <t>ue</t>
-  </si>
-  <si>
-    <t>oms</t>
-  </si>
-  <si>
-    <t>Promedio 24 horas</t>
-  </si>
-  <si>
-    <t>&lt;= 50 ug/m3; &lt;= 35 días</t>
-  </si>
-  <si>
-    <t>&lt;= 50 ug/m3; &lt;= 3 días</t>
-  </si>
-  <si>
-    <t>Promedio anual</t>
-  </si>
-  <si>
-    <t>&lt;= 40 ug/m3</t>
-  </si>
-  <si>
-    <t>&lt;= 20 ug/m3</t>
   </si>
 </sst>
 </file>
@@ -113,7 +88,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -123,9 +98,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -199,7 +171,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>arima_graph!$B$1</c:f>
+              <c:f>Sheet1!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -222,7 +194,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>arima_graph!$B$2:$B$13</c:f>
+              <c:f>Sheet1!$B$2:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -277,7 +249,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>arima_graph!$C$1</c:f>
+              <c:f>Sheet1!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -300,7 +272,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>arima_graph!$C$2:$C$13</c:f>
+              <c:f>Sheet1!$C$2:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -1442,7 +1414,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F50DCA78-E89A-4BA6-97A1-F445FBB88E11}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
@@ -1597,54 +1569,4 @@
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8264788F-3ED7-499F-95A3-F67646295472}">
-  <dimension ref="E4:G6"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
-  <cols>
-    <col min="5" max="5" width="19.1796875" customWidth="1"/>
-    <col min="6" max="6" width="20.86328125" customWidth="1"/>
-    <col min="7" max="7" width="22.1796875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="4" spans="5:7" x14ac:dyDescent="0.75">
-      <c r="F4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="5:7" x14ac:dyDescent="0.75">
-      <c r="E5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="5:7" x14ac:dyDescent="0.75">
-      <c r="E6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "Revert "Predicting PM10 hourly levels / Organizing Data Gathering and Exploration code""
This reverts commit e0ec17a2756d6135ce70beea242ff39055da0ae1.
</commit_message>
<xml_diff>
--- a/arima_prediction_graph.xlsx
+++ b/arima_prediction_graph.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/507d04ca7be29483/00_master_data_science/TFM_KSchool_Gijon_Air_Pollution/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SErgio\OneDrive\00_master_data_science\TFM_KSchool_Gijon_Air_Pollution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F038860C-ADCD-483E-99F6-B8624C407276}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="8_{F038860C-ADCD-483E-99F6-B8624C407276}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{B75EF87B-DF3F-4B5A-953E-D63ED53A25C8}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="1910" windowHeight="0" xr2:uid="{25F250B0-3884-4528-9D34-9580BA324527}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="1910" windowHeight="0" activeTab="1" xr2:uid="{25F250B0-3884-4528-9D34-9580BA324527}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="arima_graph" sheetId="1" r:id="rId1"/>
+    <sheet name="pm10_limits" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>year_month</t>
   </si>
@@ -40,6 +41,30 @@
   </si>
   <si>
     <t>real 2017</t>
+  </si>
+  <si>
+    <t>ue</t>
+  </si>
+  <si>
+    <t>oms</t>
+  </si>
+  <si>
+    <t>Promedio 24 horas</t>
+  </si>
+  <si>
+    <t>&lt;= 50 ug/m3; &lt;= 35 días</t>
+  </si>
+  <si>
+    <t>&lt;= 50 ug/m3; &lt;= 3 días</t>
+  </si>
+  <si>
+    <t>Promedio anual</t>
+  </si>
+  <si>
+    <t>&lt;= 40 ug/m3</t>
+  </si>
+  <si>
+    <t>&lt;= 20 ug/m3</t>
   </si>
 </sst>
 </file>
@@ -88,7 +113,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -98,6 +123,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -171,7 +199,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
+              <c:f>arima_graph!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -194,7 +222,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$13</c:f>
+              <c:f>arima_graph!$B$2:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -249,7 +277,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>arima_graph!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -272,7 +300,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$13</c:f>
+              <c:f>arima_graph!$C$2:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -1414,7 +1442,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F50DCA78-E89A-4BA6-97A1-F445FBB88E11}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
@@ -1569,4 +1597,54 @@
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8264788F-3ED7-499F-95A3-F67646295472}">
+  <dimension ref="E4:G6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="5" max="5" width="19.1796875" customWidth="1"/>
+    <col min="6" max="6" width="20.86328125" customWidth="1"/>
+    <col min="7" max="7" width="22.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="5:7" x14ac:dyDescent="0.75">
+      <c r="F4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="5:7" x14ac:dyDescent="0.75">
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="5:7" x14ac:dyDescent="0.75">
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>